<commit_message>
Replace . by ,
</commit_message>
<xml_diff>
--- a/datasets/la-liga-2015-2016.xlsx
+++ b/datasets/la-liga-2015-2016.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Team</t>
   </si>
@@ -39,187 +39,106 @@
     <t>Loses</t>
   </si>
   <si>
-    <t>Goals.scored</t>
-  </si>
-  <si>
-    <t>Goals.conceded</t>
-  </si>
-  <si>
-    <t>Difference.goals</t>
-  </si>
-  <si>
-    <t>Percentage.scored.goals</t>
-  </si>
-  <si>
-    <t>Percentage.conceded.goals</t>
-  </si>
-  <si>
     <t>Shots</t>
   </si>
   <si>
-    <t>Shots.on.goal</t>
-  </si>
-  <si>
-    <t>Penalties.scored</t>
-  </si>
-  <si>
     <t>Assistances</t>
   </si>
   <si>
-    <t>Fouls.made</t>
-  </si>
-  <si>
-    <t>Matches.without.conceding</t>
-  </si>
-  <si>
-    <t>Yellow.cards</t>
-  </si>
-  <si>
-    <t>Red.cards</t>
-  </si>
-  <si>
     <t>Offsides</t>
   </si>
   <si>
     <t>Barcelona</t>
   </si>
   <si>
-    <t>2.95</t>
-  </si>
-  <si>
-    <t>0.76</t>
-  </si>
-  <si>
     <t>Real Madrid</t>
   </si>
   <si>
-    <t>2.89</t>
-  </si>
-  <si>
-    <t>0.89</t>
-  </si>
-  <si>
     <t>Atlético Madrid</t>
   </si>
   <si>
-    <t>1.66</t>
-  </si>
-  <si>
-    <t>0.47</t>
-  </si>
-  <si>
     <t>Villarreal</t>
   </si>
   <si>
-    <t>1.16</t>
-  </si>
-  <si>
-    <t>0.92</t>
-  </si>
-  <si>
     <t>Athletic</t>
   </si>
   <si>
-    <t>1.53</t>
-  </si>
-  <si>
-    <t>1.18</t>
-  </si>
-  <si>
     <t>Celta</t>
   </si>
   <si>
-    <t>1.34</t>
-  </si>
-  <si>
-    <t>1.55</t>
-  </si>
-  <si>
     <t>Sevilla</t>
   </si>
   <si>
-    <t>1.32</t>
-  </si>
-  <si>
     <t>Málaga</t>
   </si>
   <si>
     <t>Real Sociedad</t>
   </si>
   <si>
-    <t>1.26</t>
-  </si>
-  <si>
     <t>Betis</t>
   </si>
   <si>
-    <t>1.37</t>
-  </si>
-  <si>
     <t>Las Palmas</t>
   </si>
   <si>
-    <t>1.39</t>
-  </si>
-  <si>
     <t>Valencia</t>
   </si>
   <si>
-    <t>1.21</t>
-  </si>
-  <si>
     <t>Eibar</t>
   </si>
   <si>
-    <t>1.29</t>
-  </si>
-  <si>
-    <t>1.61</t>
-  </si>
-  <si>
     <t>Espanyol</t>
   </si>
   <si>
-    <t>1.05</t>
-  </si>
-  <si>
-    <t>1.95</t>
-  </si>
-  <si>
     <t>Deportivo</t>
   </si>
   <si>
     <t>Granada</t>
   </si>
   <si>
-    <t>1.82</t>
-  </si>
-  <si>
     <t>Sporting Gijón</t>
   </si>
   <si>
-    <t>1.63</t>
-  </si>
-  <si>
     <t>Rayo Vallecano</t>
   </si>
   <si>
-    <t>1.92</t>
-  </si>
-  <si>
     <t>Getafe</t>
   </si>
   <si>
-    <t>0.97</t>
-  </si>
-  <si>
-    <t>1.76</t>
-  </si>
-  <si>
     <t>Levante</t>
   </si>
   <si>
-    <t>1.84</t>
+    <t>Goals,scored</t>
+  </si>
+  <si>
+    <t>Goals,conceded</t>
+  </si>
+  <si>
+    <t>Difference,goals</t>
+  </si>
+  <si>
+    <t>Percentage,scored,goals</t>
+  </si>
+  <si>
+    <t>Percentage,conceded,goals</t>
+  </si>
+  <si>
+    <t>Shots,on,goal</t>
+  </si>
+  <si>
+    <t>Penalties,scored</t>
+  </si>
+  <si>
+    <t>Fouls,made</t>
+  </si>
+  <si>
+    <t>Matches,without,conceding</t>
+  </si>
+  <si>
+    <t>Yellow,cards</t>
+  </si>
+  <si>
+    <t>Red,cards</t>
   </si>
 </sst>
 </file>
@@ -594,7 +513,7 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:T21"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -619,51 +538,51 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1">
         <v>91</v>
@@ -689,11 +608,11 @@
       <c r="I2" s="1">
         <v>83</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>22</v>
+      <c r="J2" s="1">
+        <v>2.95</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.76</v>
       </c>
       <c r="L2" s="1">
         <v>600</v>
@@ -725,7 +644,7 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1">
         <v>90</v>
@@ -751,11 +670,11 @@
       <c r="I3" s="1">
         <v>76</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>25</v>
+      <c r="J3" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.89</v>
       </c>
       <c r="L3" s="1">
         <v>712</v>
@@ -787,7 +706,7 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1">
         <v>88</v>
@@ -813,11 +732,11 @@
       <c r="I4" s="1">
         <v>45</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>28</v>
+      <c r="J4" s="1">
+        <v>1.66</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.47</v>
       </c>
       <c r="L4" s="1">
         <v>481</v>
@@ -849,7 +768,7 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1">
         <v>64</v>
@@ -875,11 +794,11 @@
       <c r="I5" s="1">
         <v>9</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>31</v>
+      <c r="J5" s="1">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.92</v>
       </c>
       <c r="L5" s="1">
         <v>346</v>
@@ -911,7 +830,7 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>62</v>
@@ -937,11 +856,11 @@
       <c r="I6" s="1">
         <v>13</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>34</v>
+      <c r="J6" s="1">
+        <v>1.53</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1.18</v>
       </c>
       <c r="L6" s="1">
         <v>450</v>
@@ -973,7 +892,7 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1">
         <v>60</v>
@@ -999,11 +918,11 @@
       <c r="I7" s="1">
         <v>-8</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>37</v>
+      <c r="J7" s="1">
+        <v>1.34</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1.55</v>
       </c>
       <c r="L7" s="1">
         <v>442</v>
@@ -1035,7 +954,7 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1">
         <v>52</v>
@@ -1061,11 +980,11 @@
       <c r="I8" s="1">
         <v>1</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>39</v>
+      <c r="J8" s="1">
+        <v>1.34</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1.32</v>
       </c>
       <c r="L8" s="1">
         <v>460</v>
@@ -1097,7 +1016,7 @@
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1">
         <v>48</v>
@@ -1126,8 +1045,8 @@
       <c r="J9" s="1">
         <v>1</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>31</v>
+      <c r="K9" s="1">
+        <v>0.92</v>
       </c>
       <c r="L9" s="1">
         <v>452</v>
@@ -1159,7 +1078,7 @@
     </row>
     <row r="10" spans="1:20">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1">
         <v>48</v>
@@ -1185,11 +1104,11 @@
       <c r="I10" s="1">
         <v>-3</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>42</v>
+      <c r="J10" s="1">
+        <v>1.18</v>
+      </c>
+      <c r="K10" s="1">
+        <v>1.26</v>
       </c>
       <c r="L10" s="1">
         <v>454</v>
@@ -1221,7 +1140,7 @@
     </row>
     <row r="11" spans="1:20">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1">
         <v>45</v>
@@ -1247,11 +1166,11 @@
       <c r="I11" s="1">
         <v>-18</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>44</v>
+      <c r="J11" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1.37</v>
       </c>
       <c r="L11" s="1">
         <v>398</v>
@@ -1283,7 +1202,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1">
         <v>44</v>
@@ -1309,11 +1228,11 @@
       <c r="I12" s="1">
         <v>-8</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>46</v>
+      <c r="J12" s="1">
+        <v>1.18</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1.39</v>
       </c>
       <c r="L12" s="1">
         <v>418</v>
@@ -1345,7 +1264,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1">
         <v>44</v>
@@ -1371,11 +1290,11 @@
       <c r="I13" s="1">
         <v>-2</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>42</v>
+      <c r="J13" s="1">
+        <v>1.21</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1.26</v>
       </c>
       <c r="L13" s="1">
         <v>401</v>
@@ -1407,7 +1326,7 @@
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="1" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1">
         <v>43</v>
@@ -1433,11 +1352,11 @@
       <c r="I14" s="1">
         <v>-12</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>51</v>
+      <c r="J14" s="1">
+        <v>1.29</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1.61</v>
       </c>
       <c r="L14" s="1">
         <v>421</v>
@@ -1469,7 +1388,7 @@
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="1" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1">
         <v>43</v>
@@ -1495,11 +1414,11 @@
       <c r="I15" s="1">
         <v>-34</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>54</v>
+      <c r="J15" s="1">
+        <v>1.05</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1.95</v>
       </c>
       <c r="L15" s="1">
         <v>388</v>
@@ -1531,7 +1450,7 @@
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="1" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1">
         <v>42</v>
@@ -1557,11 +1476,11 @@
       <c r="I16" s="1">
         <v>-16</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>51</v>
+      <c r="J16" s="1">
+        <v>1.18</v>
+      </c>
+      <c r="K16" s="1">
+        <v>1.61</v>
       </c>
       <c r="L16" s="1">
         <v>451</v>
@@ -1593,7 +1512,7 @@
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="1" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1">
         <v>39</v>
@@ -1619,11 +1538,11 @@
       <c r="I17" s="1">
         <v>-23</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>57</v>
+      <c r="J17" s="1">
+        <v>1.21</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1.82</v>
       </c>
       <c r="L17" s="1">
         <v>430</v>
@@ -1655,7 +1574,7 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="1" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1">
         <v>39</v>
@@ -1681,11 +1600,11 @@
       <c r="I18" s="1">
         <v>-22</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>59</v>
+      <c r="J18" s="1">
+        <v>1.05</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1.63</v>
       </c>
       <c r="L18" s="1">
         <v>372</v>
@@ -1717,7 +1636,7 @@
     </row>
     <row r="19" spans="1:20">
       <c r="A19" s="1" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="B19" s="1">
         <v>38</v>
@@ -1743,11 +1662,11 @@
       <c r="I19" s="1">
         <v>-21</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>61</v>
+      <c r="J19" s="1">
+        <v>1.37</v>
+      </c>
+      <c r="K19" s="1">
+        <v>1.92</v>
       </c>
       <c r="L19" s="1">
         <v>505</v>
@@ -1779,7 +1698,7 @@
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="B20" s="1">
         <v>36</v>
@@ -1805,11 +1724,11 @@
       <c r="I20" s="1">
         <v>-30</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>64</v>
+      <c r="J20" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="K20" s="1">
+        <v>1.76</v>
       </c>
       <c r="L20" s="1">
         <v>433</v>
@@ -1841,7 +1760,7 @@
     </row>
     <row r="21" spans="1:20">
       <c r="A21" s="1" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="B21" s="1">
         <v>32</v>
@@ -1867,11 +1786,11 @@
       <c r="I21" s="1">
         <v>-33</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>66</v>
+      <c r="J21" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="K21" s="1">
+        <v>1.84</v>
       </c>
       <c r="L21" s="1">
         <v>434</v>

</xml_diff>